<commit_message>
Version 1.1 Excel Trigger Regression
</commit_message>
<xml_diff>
--- a/ace_testlist_ttlhg4_v1.xlsx
+++ b/ace_testlist_ttlhg4_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcfsv01a-cifs.png.intel.com\png_viceipr_disk001\FalconRun\users\QUAL\Hardening_test\Automation-Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932AD216-605E-403F-8247-D0EFD850560E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4335FBE1-9302-4E7E-94BB-E0D3A4DEAEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6481,7 +6481,7 @@
   <dimension ref="A1:N1266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D776" sqref="D776"/>
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -8553,9 +8553,9 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
@@ -8901,7 +8901,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="b">
         <v>0</v>
       </c>
@@ -10321,7 +10321,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="b">
         <v>0</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="b">
         <v>0</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="b">
         <v>0</v>
       </c>
@@ -15676,7 +15676,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A390" s="2" t="b">
         <v>0</v>
       </c>
@@ -16581,7 +16581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A427" s="2" t="b">
         <v>0</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A447" s="2" t="b">
         <v>0</v>
       </c>
@@ -17505,7 +17505,7 @@
     </row>
     <row r="465" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A465" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B465" t="s">
         <v>14</v>
@@ -18736,7 +18736,7 @@
     </row>
     <row r="512" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A512" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B512" t="s">
         <v>14</v>
@@ -19135,7 +19135,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="528" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="528" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A528" s="2" t="b">
         <v>0</v>
       </c>
@@ -25071,7 +25071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="763" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="763" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A763" s="2" t="b">
         <v>0</v>
       </c>
@@ -25097,7 +25097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="764" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="764" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A764" s="2" t="b">
         <v>0</v>
       </c>
@@ -25123,9 +25123,9 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="765" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="765" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A765" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B765" t="s">
         <v>14</v>
@@ -25152,7 +25152,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="766" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="766" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A766" s="2" t="b">
         <v>0</v>
       </c>
@@ -25178,7 +25178,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="767" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="767" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A767" s="2" t="b">
         <v>0</v>
       </c>
@@ -25204,7 +25204,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="768" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="768" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A768" s="2" t="b">
         <v>0</v>
       </c>
@@ -25230,9 +25230,9 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="769" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="769" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A769" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B769" t="s">
         <v>14</v>
@@ -25259,7 +25259,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="770" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="770" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A770" s="2" t="b">
         <v>0</v>
       </c>
@@ -25288,7 +25288,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="771" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="771" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A771" s="2" t="b">
         <v>0</v>
       </c>
@@ -25314,7 +25314,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="772" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="772" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A772" s="2" t="b">
         <v>0</v>
       </c>
@@ -25343,7 +25343,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="773" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="773" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A773" s="2" t="b">
         <v>0</v>
       </c>
@@ -25372,7 +25372,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="774" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="774" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A774" s="2" t="b">
         <v>0</v>
       </c>
@@ -25401,7 +25401,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="775" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="775" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A775" s="2" t="b">
         <v>0</v>
       </c>
@@ -25432,7 +25432,7 @@
     </row>
     <row r="776" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A776" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B776" t="s">
         <v>14</v>
@@ -25459,7 +25459,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="777" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="777" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A777" s="2" t="b">
         <v>0</v>
       </c>
@@ -25485,7 +25485,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="778" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="778" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A778" s="2" t="b">
         <v>0</v>
       </c>
@@ -25511,7 +25511,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="779" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="779" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A779" s="2" t="b">
         <v>0</v>
       </c>
@@ -25537,7 +25537,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="780" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="780" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A780" s="2" t="b">
         <v>0</v>
       </c>
@@ -25563,7 +25563,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="781" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="781" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A781" s="2" t="b">
         <v>0</v>
       </c>
@@ -25592,7 +25592,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="782" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="782" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A782" s="2" t="b">
         <v>0</v>
       </c>
@@ -25618,7 +25618,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="783" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="783" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A783" s="2" t="b">
         <v>0</v>
       </c>
@@ -25647,7 +25647,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="784" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="784" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A784" s="2" t="b">
         <v>0</v>
       </c>
@@ -25676,7 +25676,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="785" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="785" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A785" s="2" t="b">
         <v>0</v>
       </c>
@@ -25705,7 +25705,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="786" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="786" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A786" s="2" t="b">
         <v>0</v>
       </c>
@@ -25731,7 +25731,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="787" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="787" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A787" s="2" t="b">
         <v>0</v>
       </c>
@@ -25760,7 +25760,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="788" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="788" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A788" s="2" t="b">
         <v>0</v>
       </c>
@@ -25789,7 +25789,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="789" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="789" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A789" s="2" t="b">
         <v>0</v>
       </c>
@@ -25818,7 +25818,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="790" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="790" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A790" s="2" t="b">
         <v>0</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="791" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="791" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A791" s="2" t="b">
         <v>0</v>
       </c>
@@ -25876,7 +25876,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="792" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="792" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A792" s="2" t="b">
         <v>0</v>
       </c>
@@ -25905,7 +25905,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="793" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="793" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A793" s="2" t="b">
         <v>0</v>
       </c>
@@ -25931,7 +25931,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="794" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="794" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A794" s="2" t="b">
         <v>0</v>
       </c>
@@ -25960,7 +25960,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="795" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="795" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A795" s="2" t="b">
         <v>0</v>
       </c>
@@ -25989,7 +25989,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="796" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="796" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A796" s="2" t="b">
         <v>0</v>
       </c>
@@ -26018,7 +26018,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="797" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="797" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A797" s="2" t="b">
         <v>0</v>
       </c>
@@ -26044,7 +26044,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="798" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="798" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A798" s="2" t="b">
         <v>0</v>
       </c>
@@ -26073,7 +26073,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="799" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="799" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A799" s="2" t="b">
         <v>0</v>
       </c>
@@ -26102,7 +26102,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="800" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="800" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A800" s="2" t="b">
         <v>0</v>
       </c>
@@ -26131,7 +26131,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="801" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="801" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A801" s="2" t="b">
         <v>0</v>
       </c>
@@ -26160,7 +26160,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="802" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="802" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A802" s="2" t="b">
         <v>0</v>
       </c>
@@ -26189,7 +26189,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="803" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="803" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A803" s="2" t="b">
         <v>0</v>
       </c>
@@ -26218,7 +26218,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="804" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="804" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A804" s="2" t="b">
         <v>0</v>
       </c>
@@ -26244,7 +26244,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="805" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="805" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A805" s="2" t="b">
         <v>0</v>
       </c>
@@ -26273,7 +26273,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="806" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="806" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A806" s="2" t="b">
         <v>0</v>
       </c>
@@ -26299,7 +26299,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="807" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="807" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A807" s="2" t="b">
         <v>0</v>
       </c>
@@ -26328,7 +26328,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="808" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="808" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A808" s="2" t="b">
         <v>0</v>
       </c>
@@ -26354,7 +26354,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="809" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="809" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A809" s="2" t="b">
         <v>0</v>
       </c>
@@ -26383,7 +26383,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="810" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="810" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A810" s="2" t="b">
         <v>0</v>
       </c>
@@ -26409,7 +26409,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="811" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="811" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A811" s="2" t="b">
         <v>0</v>
       </c>
@@ -26438,7 +26438,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="812" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="812" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A812" s="2" t="b">
         <v>0</v>
       </c>
@@ -26464,7 +26464,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="813" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="813" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A813" s="2" t="b">
         <v>0</v>
       </c>
@@ -26493,7 +26493,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="814" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="814" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A814" s="2" t="b">
         <v>0</v>
       </c>
@@ -26519,7 +26519,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="815" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="815" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A815" s="2" t="b">
         <v>0</v>
       </c>
@@ -26548,7 +26548,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="816" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="816" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A816" s="2" t="b">
         <v>0</v>
       </c>
@@ -26574,7 +26574,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="817" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="817" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A817" s="2" t="b">
         <v>0</v>
       </c>
@@ -26600,7 +26600,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="818" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="818" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A818" s="2" t="b">
         <v>0</v>
       </c>
@@ -26629,7 +26629,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="819" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="819" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A819" s="2" t="b">
         <v>0</v>
       </c>
@@ -26658,7 +26658,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="820" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="820" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A820" s="2" t="b">
         <v>0</v>
       </c>
@@ -26687,7 +26687,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="821" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="821" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A821" s="2" t="b">
         <v>0</v>
       </c>
@@ -26716,7 +26716,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="822" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="822" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A822" s="2" t="b">
         <v>0</v>
       </c>
@@ -26742,7 +26742,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="823" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="823" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A823" s="2" t="b">
         <v>0</v>
       </c>
@@ -26768,7 +26768,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="824" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="824" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A824" s="2" t="b">
         <v>0</v>
       </c>
@@ -26794,7 +26794,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="825" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="825" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A825" s="2" t="b">
         <v>0</v>
       </c>
@@ -26820,7 +26820,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="826" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="826" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A826" s="2" t="b">
         <v>0</v>
       </c>
@@ -26846,7 +26846,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="827" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="827" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A827" s="2" t="b">
         <v>0</v>
       </c>
@@ -26872,7 +26872,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="828" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="828" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A828" s="2" t="b">
         <v>0</v>
       </c>
@@ -26898,7 +26898,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="829" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="829" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A829" s="2" t="b">
         <v>0</v>
       </c>
@@ -26924,7 +26924,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="830" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="830" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A830" s="2" t="b">
         <v>0</v>
       </c>
@@ -26950,7 +26950,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="831" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="831" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A831" s="2" t="b">
         <v>0</v>
       </c>
@@ -26976,7 +26976,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="832" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="832" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A832" s="2" t="b">
         <v>0</v>
       </c>
@@ -27002,7 +27002,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="833" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="833" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A833" s="2" t="b">
         <v>0</v>
       </c>
@@ -27028,7 +27028,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="834" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="834" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A834" s="2" t="b">
         <v>0</v>
       </c>
@@ -27054,7 +27054,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="835" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="835" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A835" s="2" t="b">
         <v>0</v>
       </c>
@@ -27080,7 +27080,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="836" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="836" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A836" s="2" t="b">
         <v>0</v>
       </c>
@@ -27106,7 +27106,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="837" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="837" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A837" s="2" t="b">
         <v>0</v>
       </c>
@@ -27132,7 +27132,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="838" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="838" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A838" s="2" t="b">
         <v>0</v>
       </c>
@@ -27158,7 +27158,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="839" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="839" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A839" s="2" t="b">
         <v>0</v>
       </c>
@@ -27184,7 +27184,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="840" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="840" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A840" s="2" t="b">
         <v>0</v>
       </c>
@@ -27210,7 +27210,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="841" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="841" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A841" s="2" t="b">
         <v>0</v>
       </c>
@@ -27236,7 +27236,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="842" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="842" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A842" s="2" t="b">
         <v>0</v>
       </c>
@@ -27262,7 +27262,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="843" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="843" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A843" s="2" t="b">
         <v>0</v>
       </c>
@@ -27288,7 +27288,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="844" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="844" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A844" s="2" t="b">
         <v>0</v>
       </c>
@@ -27314,7 +27314,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="845" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="845" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A845" s="2" t="b">
         <v>0</v>
       </c>
@@ -27340,7 +27340,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="846" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="846" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A846" s="2" t="b">
         <v>0</v>
       </c>
@@ -27366,7 +27366,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="847" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="847" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A847" s="2" t="b">
         <v>0</v>
       </c>
@@ -27392,7 +27392,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="848" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="848" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A848" s="2" t="b">
         <v>0</v>
       </c>
@@ -27418,7 +27418,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="849" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="849" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A849" s="2" t="b">
         <v>0</v>
       </c>
@@ -27444,7 +27444,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="850" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="850" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A850" s="2" t="b">
         <v>0</v>
       </c>
@@ -27470,7 +27470,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="851" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="851" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A851" s="2" t="b">
         <v>0</v>
       </c>
@@ -27496,7 +27496,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="852" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="852" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A852" s="2" t="b">
         <v>0</v>
       </c>
@@ -27522,7 +27522,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="853" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="853" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A853" s="2" t="b">
         <v>0</v>
       </c>
@@ -27548,7 +27548,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="854" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="854" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A854" s="2" t="b">
         <v>0</v>
       </c>
@@ -27574,7 +27574,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="855" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="855" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A855" s="2" t="b">
         <v>0</v>
       </c>
@@ -27600,7 +27600,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="856" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="856" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A856" s="2" t="b">
         <v>0</v>
       </c>
@@ -27626,7 +27626,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="857" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="857" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A857" s="2" t="b">
         <v>0</v>
       </c>
@@ -27652,7 +27652,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="858" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="858" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A858" s="2" t="b">
         <v>0</v>
       </c>
@@ -27678,7 +27678,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="859" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="859" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A859" s="2" t="b">
         <v>0</v>
       </c>
@@ -27704,7 +27704,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="860" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="860" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A860" s="2" t="b">
         <v>0</v>
       </c>
@@ -27730,7 +27730,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="861" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="861" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A861" s="2" t="b">
         <v>0</v>
       </c>
@@ -27756,7 +27756,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="862" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="862" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A862" s="2" t="b">
         <v>0</v>
       </c>
@@ -27782,7 +27782,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="863" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="863" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A863" s="2" t="b">
         <v>0</v>
       </c>
@@ -27808,7 +27808,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="864" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="864" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A864" s="2" t="b">
         <v>0</v>
       </c>
@@ -27834,7 +27834,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="865" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="865" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A865" s="2" t="b">
         <v>0</v>
       </c>
@@ -27860,7 +27860,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="866" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="866" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A866" s="2" t="b">
         <v>0</v>
       </c>
@@ -27886,7 +27886,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="867" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="867" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A867" s="2" t="b">
         <v>0</v>
       </c>
@@ -27912,7 +27912,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="868" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="868" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A868" s="2" t="b">
         <v>0</v>
       </c>
@@ -27938,7 +27938,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="869" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="869" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A869" s="2" t="b">
         <v>0</v>
       </c>
@@ -27964,7 +27964,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="870" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="870" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A870" s="2" t="b">
         <v>0</v>
       </c>
@@ -27990,7 +27990,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="871" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="871" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A871" s="2" t="b">
         <v>0</v>
       </c>
@@ -28016,7 +28016,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="872" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="872" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A872" s="2" t="b">
         <v>0</v>
       </c>
@@ -28042,7 +28042,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="873" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="873" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A873" s="2" t="b">
         <v>0</v>
       </c>
@@ -28071,7 +28071,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="874" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="874" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A874" s="2" t="b">
         <v>0</v>
       </c>
@@ -28097,7 +28097,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="875" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="875" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A875" s="2" t="b">
         <v>0</v>
       </c>
@@ -28123,7 +28123,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="876" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="876" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A876" s="2" t="b">
         <v>0</v>
       </c>
@@ -28149,7 +28149,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="877" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="877" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A877" s="2" t="b">
         <v>0</v>
       </c>
@@ -28178,7 +28178,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="878" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="878" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A878" s="2" t="b">
         <v>0</v>
       </c>
@@ -28207,7 +28207,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="879" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="879" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A879" s="2" t="b">
         <v>0</v>
       </c>
@@ -28233,7 +28233,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="880" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="880" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A880" s="2" t="b">
         <v>0</v>
       </c>
@@ -28262,7 +28262,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="881" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="881" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A881" s="2" t="b">
         <v>0</v>
       </c>
@@ -28291,7 +28291,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="882" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="882" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A882" s="2" t="b">
         <v>0</v>
       </c>
@@ -28320,7 +28320,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="883" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="883" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A883" s="2" t="b">
         <v>0</v>
       </c>
@@ -28349,7 +28349,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="884" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="884" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A884" s="2" t="b">
         <v>0</v>
       </c>
@@ -28378,7 +28378,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="885" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="885" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A885" s="2" t="b">
         <v>0</v>
       </c>
@@ -28404,7 +28404,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="886" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="886" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A886" s="2" t="b">
         <v>0</v>
       </c>
@@ -28430,7 +28430,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="887" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="887" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A887" s="2" t="b">
         <v>0</v>
       </c>
@@ -28456,7 +28456,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="888" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="888" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A888" s="2" t="b">
         <v>0</v>
       </c>
@@ -28482,7 +28482,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="889" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="889" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A889" s="2" t="b">
         <v>0</v>
       </c>
@@ -28511,7 +28511,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="890" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="890" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A890" s="2" t="b">
         <v>0</v>
       </c>
@@ -28537,7 +28537,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="891" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="891" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A891" s="2" t="b">
         <v>0</v>
       </c>
@@ -28566,7 +28566,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="892" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="892" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A892" s="2" t="b">
         <v>0</v>
       </c>
@@ -28595,7 +28595,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="893" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="893" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A893" s="2" t="b">
         <v>0</v>
       </c>
@@ -28624,7 +28624,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="894" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="894" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A894" s="2" t="b">
         <v>0</v>
       </c>
@@ -28650,7 +28650,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="895" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="895" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A895" s="2" t="b">
         <v>0</v>
       </c>
@@ -28679,7 +28679,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="896" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="896" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A896" s="2" t="b">
         <v>0</v>
       </c>
@@ -28708,7 +28708,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="897" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="897" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A897" s="2" t="b">
         <v>0</v>
       </c>
@@ -28737,7 +28737,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="898" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="898" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A898" s="2" t="b">
         <v>0</v>
       </c>
@@ -28766,7 +28766,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="899" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="899" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A899" s="2" t="b">
         <v>0</v>
       </c>
@@ -28795,7 +28795,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="900" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="900" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A900" s="2" t="b">
         <v>0</v>
       </c>
@@ -28824,7 +28824,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="901" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="901" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A901" s="2" t="b">
         <v>0</v>
       </c>
@@ -28850,7 +28850,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="902" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="902" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A902" s="2" t="b">
         <v>0</v>
       </c>
@@ -28879,7 +28879,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="903" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="903" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A903" s="2" t="b">
         <v>0</v>
       </c>
@@ -28908,7 +28908,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="904" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="904" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A904" s="2" t="b">
         <v>0</v>
       </c>
@@ -28937,7 +28937,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="905" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="905" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A905" s="2" t="b">
         <v>0</v>
       </c>
@@ -28963,7 +28963,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="906" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="906" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A906" s="2" t="b">
         <v>0</v>
       </c>
@@ -28992,7 +28992,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="907" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="907" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A907" s="2" t="b">
         <v>0</v>
       </c>
@@ -29021,7 +29021,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="908" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="908" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A908" s="2" t="b">
         <v>0</v>
       </c>
@@ -29050,7 +29050,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="909" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="909" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A909" s="2" t="b">
         <v>0</v>
       </c>
@@ -29079,7 +29079,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="910" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="910" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A910" s="2" t="b">
         <v>0</v>
       </c>
@@ -29108,7 +29108,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="911" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="911" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A911" s="2" t="b">
         <v>0</v>
       </c>
@@ -29137,7 +29137,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="912" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="912" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A912" s="2" t="b">
         <v>0</v>
       </c>
@@ -29163,7 +29163,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="913" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="913" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A913" s="2" t="b">
         <v>0</v>
       </c>
@@ -29192,7 +29192,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="914" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="914" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A914" s="2" t="b">
         <v>0</v>
       </c>
@@ -29218,7 +29218,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="915" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="915" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A915" s="2" t="b">
         <v>0</v>
       </c>
@@ -29247,7 +29247,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="916" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="916" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A916" s="2" t="b">
         <v>0</v>
       </c>
@@ -29273,7 +29273,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="917" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="917" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A917" s="2" t="b">
         <v>0</v>
       </c>
@@ -29302,7 +29302,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="918" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="918" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A918" s="2" t="b">
         <v>0</v>
       </c>
@@ -29328,7 +29328,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="919" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="919" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A919" s="2" t="b">
         <v>0</v>
       </c>
@@ -29357,7 +29357,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="920" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="920" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A920" s="2" t="b">
         <v>0</v>
       </c>
@@ -29383,7 +29383,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="921" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="921" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A921" s="2" t="b">
         <v>0</v>
       </c>
@@ -29412,7 +29412,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="922" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="922" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A922" s="2" t="b">
         <v>0</v>
       </c>
@@ -29438,7 +29438,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="923" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="923" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A923" s="2" t="b">
         <v>0</v>
       </c>
@@ -29467,7 +29467,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="924" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="924" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A924" s="2" t="b">
         <v>0</v>
       </c>
@@ -29493,7 +29493,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="925" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="925" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A925" s="2" t="b">
         <v>0</v>
       </c>
@@ -29522,7 +29522,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="926" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="926" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A926" s="2" t="b">
         <v>0</v>
       </c>
@@ -29548,7 +29548,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="927" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="927" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A927" s="2" t="b">
         <v>0</v>
       </c>
@@ -29574,7 +29574,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="928" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="928" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A928" s="2" t="b">
         <v>0</v>
       </c>
@@ -29603,7 +29603,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="929" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="929" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A929" s="2" t="b">
         <v>0</v>
       </c>
@@ -29632,7 +29632,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="930" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="930" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A930" s="2" t="b">
         <v>0</v>
       </c>
@@ -29661,7 +29661,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="931" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="931" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A931" s="2" t="b">
         <v>0</v>
       </c>
@@ -29690,7 +29690,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="932" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="932" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A932" s="2" t="b">
         <v>0</v>
       </c>
@@ -29716,7 +29716,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="933" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="933" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A933" s="2" t="b">
         <v>0</v>
       </c>
@@ -31782,7 +31782,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="1030" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1030" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1030" s="2" t="b">
         <v>0</v>
       </c>
@@ -34741,7 +34741,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="1167" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1167" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1167" s="2" t="b">
         <v>0</v>
       </c>
@@ -34764,7 +34764,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1168" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1168" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1168" s="2" t="b">
         <v>0</v>
       </c>
@@ -34867,7 +34867,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1173" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1173" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1173" s="2" t="b">
         <v>0</v>
       </c>
@@ -34910,7 +34910,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="1175" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1175" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1175" s="2" t="b">
         <v>0</v>
       </c>
@@ -34953,7 +34953,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="1177" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1177" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1177" s="2" t="b">
         <v>0</v>
       </c>
@@ -34976,7 +34976,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="1178" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1178" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1178" s="2" t="b">
         <v>0</v>
       </c>
@@ -35019,7 +35019,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1180" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1180" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1180" s="2" t="b">
         <v>0</v>
       </c>
@@ -35128,7 +35128,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="1185" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1185" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1185" s="2" t="b">
         <v>0</v>
       </c>
@@ -35151,7 +35151,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="1186" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1186" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1186" s="2" t="b">
         <v>0</v>
       </c>
@@ -35174,7 +35174,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1187" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1187" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1187" s="2" t="b">
         <v>0</v>
       </c>
@@ -35197,7 +35197,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1188" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1188" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1188" s="2" t="b">
         <v>0</v>
       </c>
@@ -35220,7 +35220,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1189" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1189" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1189" s="2" t="b">
         <v>0</v>
       </c>
@@ -35243,7 +35243,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="1190" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1190" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1190" s="2" t="b">
         <v>0</v>
       </c>
@@ -35266,7 +35266,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="1191" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1191" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1191" s="2" t="b">
         <v>0</v>
       </c>
@@ -35289,7 +35289,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="1192" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1192" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1192" s="2" t="b">
         <v>0</v>
       </c>
@@ -35332,7 +35332,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="1194" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1194" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1194" s="2" t="b">
         <v>0</v>
       </c>
@@ -36231,7 +36231,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="1237" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1237" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1237" s="2" t="b">
         <v>0</v>
       </c>
@@ -36254,7 +36254,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1238" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1238" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1238" s="2" t="b">
         <v>0</v>
       </c>
@@ -36277,7 +36277,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1239" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1239" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1239" s="2" t="b">
         <v>0</v>
       </c>
@@ -36300,7 +36300,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1240" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1240" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1240" s="2" t="b">
         <v>0</v>
       </c>
@@ -36323,7 +36323,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1241" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1241" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1241" s="2" t="b">
         <v>0</v>
       </c>
@@ -36346,7 +36346,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1242" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1242" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1242" s="2" t="b">
         <v>0</v>
       </c>
@@ -36369,7 +36369,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1243" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1243" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1243" s="2" t="b">
         <v>0</v>
       </c>
@@ -36392,7 +36392,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1244" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1244" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1244" s="2" t="b">
         <v>0</v>
       </c>
@@ -36415,7 +36415,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1245" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1245" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1245" s="2" t="b">
         <v>0</v>
       </c>
@@ -36438,7 +36438,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1246" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1246" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1246" s="2" t="b">
         <v>0</v>
       </c>
@@ -36461,7 +36461,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1247" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1247" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1247" s="2" t="b">
         <v>0</v>
       </c>
@@ -36484,7 +36484,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="1248" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1248" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1248" s="2" t="b">
         <v>0</v>
       </c>
@@ -36507,7 +36507,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1249" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1249" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1249" s="2" t="b">
         <v>0</v>
       </c>
@@ -36530,7 +36530,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1250" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1250" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1250" s="2" t="b">
         <v>0</v>
       </c>
@@ -36553,7 +36553,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1251" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1251" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1251" s="2" t="b">
         <v>0</v>
       </c>
@@ -36576,7 +36576,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1252" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1252" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1252" s="2" t="b">
         <v>0</v>
       </c>
@@ -36599,7 +36599,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1253" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1253" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1253" s="2" t="b">
         <v>0</v>
       </c>
@@ -36622,7 +36622,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1254" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1254" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1254" s="2" t="b">
         <v>0</v>
       </c>
@@ -36645,7 +36645,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1255" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1255" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1255" s="2" t="b">
         <v>0</v>
       </c>
@@ -36751,7 +36751,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="1260" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1260" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1260" s="2" t="b">
         <v>0</v>
       </c>
@@ -36899,14 +36899,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N1266" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
+    <filterColumn colId="2">
       <filters>
-        <filter val="perspec_maestro"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="/nfs/png/disks/png_coesv_disk001/Platform_Bling/PGVICEWINCIcommon.bl"/>
+        <filter val="ADSP"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>